<commit_message>
Atualização do trabalho final
</commit_message>
<xml_diff>
--- a/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
+++ b/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0036D67-6F01-494A-90D1-70D461368E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C158FE91-C756-A94D-B3BF-A5FF013163AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="-17460" windowWidth="24940" windowHeight="14980" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
+    <workbookView xWindow="320" yWindow="800" windowWidth="24940" windowHeight="14980" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>@article{article,
 author = {Rossel, Pierre},
@@ -99,7 +99,29 @@
     <t>Exploring the weak signals of start-ups as a folksonomic system</t>
   </si>
   <si>
-    <t>O autor questiona como seria possível analisar tendencias emergentes através das estratégias de determinados atores acerca do futuro. Assim, ele prossegue questionando, como seria possível que sinais antecipativos de novas tendências apareçam em um campo que não está formalmente estabilizado? A hipótese colocada pelo autor é que os sinais antecipativos de mudanças futuras não são encontrados em sua forma integra (em inglês ele coloca "are not given once and for all"), mas existem internamente em processos constantes de mudança e poderiam ser mapeados através de mapas de folksonomia (citar o que é).</t>
+    <t xml:space="preserve">O autor questiona como seria possível analisar tendencias emergentes através das estratégias de determinados atores acerca do futuro. Assim, ele prossegue questionando, como seria possível que sinais antecipativos de novas tendências apareçam em um campo que não está formalmente estabilizado? A hipótese colocada pelo autor é que os sinais antecipativos de mudanças futuras não são encontrados em sua forma integra (em inglês ele coloca "are not given once and for all"), mas existem internamente em processos constantes de mudança e poderiam ser mapeados através de mapas de folksonomia (citar o que é). Através de uma pesquisa feita em sites que possuem tags de caracterização para algumas start-ups, os autores fizeram um levantamento de evolução desses termos (tags) ao longo de 2005 e 2007 com fins de verificar como os mesmos termos evoluem do passado (2005) para o futuro (2007), verificando quais eram os seus significados e como eles se desenvolveram. </t>
+  </si>
+  <si>
+    <t>Verificar como as tags são evoluídas e como seus significados se modificam ao longo do tempo.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Liebl, Franz and Schwarz, Jan Oliver},
+year = {2010},
+month = {05},
+pages = {313-327},
+title = {Normality of the future: Trend diagnosis for strategic foresight},
+volume = {42},
+journal = {Futures},
+doi = {10.1016/j.futures.2009.11.017}
+}</t>
+  </si>
+  <si>
+    <t>Jan Oliver Schwarz
+Franz Liebl</t>
+  </si>
+  <si>
+    <t>Normality of the future: Trend diagnosis for strategic foresight</t>
   </si>
 </sst>
 </file>
@@ -475,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5CE23C-BB8F-374F-A4F3-25FE445B638E}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -537,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="195" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -550,8 +572,22 @@
       <c r="D3" s="4">
         <v>2009</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="150" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primeira versão da dissertação para qualificação.
</commit_message>
<xml_diff>
--- a/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
+++ b/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C158FE91-C756-A94D-B3BF-A5FF013163AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C02841-CBFD-8542-AAA3-932085ED817A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="800" windowWidth="24940" windowHeight="14980" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$H$26</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
   <si>
     <t>@article{article,
 author = {Rossel, Pierre},
@@ -117,18 +120,581 @@
 }</t>
   </si>
   <si>
-    <t>Jan Oliver Schwarz
-Franz Liebl</t>
-  </si>
-  <si>
     <t>Normality of the future: Trend diagnosis for strategic foresight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os autores buscam com o seu trabalho sanar o problema de difusão de uma determinada tendência. Segundo os autores, apesar dos sinais fracos tratarem de tendências, existe um "gap" nos trabalhos científicos de como tratar os sinais fracos que gerariam uma tendência com fins de disseminá-lo como algo novo (inovador). Assim eles pretendem elaborar um framework para para identificar o caráter inovador das tendências e operacionalizar uma forma de disseminação dessa tendência. </t>
+  </si>
+  <si>
+    <t>Como fazer para que uma tendência seja disseminada.</t>
+  </si>
+  <si>
+    <t>@inproceedings{inproceedings,
+author = {Steinecke, Neon and Quick, Reiner and Mohr, Thomas},
+year = {2011},
+month = {01},
+pages = {181},
+title = {Environmental Scanning Systems: State Of The Art And First Instantiation.},
+journal = {PACIS 2011 - 15th Pacific Asia Conference on Information Systems: Quality Research in Pacific}
+}</t>
+  </si>
+  <si>
+    <t>Envoironmental Scanning Systems: State Of The Art And First Instantiation</t>
+  </si>
+  <si>
+    <t>Os autores propõem uma revisão de literatura para verificar achados voltados para a implementação de ESS (Environmental Scanning Systems, sigla em inglês para Sistemas de Escaneamento Ambiental). Os autores apresentam seis proposituras (5 aplicações de sistema e uma implementação): o primeiro para ser aplicado dentro de uma organização a fim de verificar qual é a melhor área para se escanear e manter foco; outros três achados são voltados para análise de sinais fracos; um outro achado voltado para incorporação de resultados desses escaneamentos no processo de tomada de decisão das organizações; e, por fim, a implementação em uma empresa para verificação dos resultados.</t>
+  </si>
+  <si>
+    <t>A methodology of technological foresight: A proposal and field study</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Battistella, Cinzia and De Toni, Alberto},
+year = {2011},
+month = {07},
+pages = {1029-1048},
+title = {A methodology of technological foresight: A proposal and field study},
+volume = {78},
+journal = {Technological Forecasting and Social Change - TECHNOL FORECAST SOC CHANGE},
+doi = {10.1016/j.techfore.2011.01.006}
+}</t>
+  </si>
+  <si>
+    <t>Jan Oliver Schwarz, Franz Liebl</t>
+  </si>
+  <si>
+    <t>Neon Conner Steinecke, Reiner Quick, Thomas Mohr</t>
+  </si>
+  <si>
+    <t>Cinzia Battistella, Alberto F. De Toni</t>
+  </si>
+  <si>
+    <t>Revisão de literatura voltada a algumas possíveis implementações de ESS</t>
+  </si>
+  <si>
+    <t>Os autores informam que a literatura existente atualmente não provê metodologias completas e bem definidas para analisar a coerencia entre tendências, visões e produtos. Assim os autores propões uma metodologia, chamada de "metodologia de cobertura de futuro" a qual mede o quanto a estratégia orientada para o futuro efetivamente cobre tendêcias e megatendências. Em outras palavras, essa metodologia ajuda a verificar a visão da empresa e seus produtos em conjunto com as tendências que seriam relevantes para o futuro da organização. Segundo os autores informam, a metologia tem a possibilidade de diagnosticar a coerência entre tendências e a estratégia da compahnia.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Comai, Alessandro},
+year = {2011},
+month = {09},
+pages = {489-494},
+title = {Inteligencia competitiva: Logros y desafíos},
+volume = {20},
+journal = {El Profesional de la Informacion},
+doi = {10.3145/epi.2011.sep.01}
+}</t>
+  </si>
+  <si>
+    <t>Alessandro Comai</t>
+  </si>
+  <si>
+    <t>Inteligencia competitiva: Logros y desafíos</t>
+  </si>
+  <si>
+    <t>Criação de uma metodologia para verificar a aderência da estratégia de uma empresa com as tendências e estratégias que a compahnia busca.</t>
+  </si>
+  <si>
+    <t>O autor busca demonstrar as questões mais críticas e possíveis problemas que podem aparecer durante a implementação de inteligência competitiva dentro de uma organização. O autor reitera que um dos pontos que podem ser abordados de inteligência competitiva é a "inteligência online" que são software que fazem busca de sinais antecipativos e que a sua grande maioria utiliza para essa finalidade o google, além de que exige um grande esforço por parte da empresa com a intenção de possuir recursos humanos, tecnológicos e financeiros,  treinar o usuário a analisar as informações que são recuperadas.</t>
+  </si>
+  <si>
+    <t>Quais são os possíveis problemas enfrentado por uma empresa para implementar IC</t>
+  </si>
+  <si>
+    <t>Content Accessibility and Semantic Networks Processed on Foreign Natural Language Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernard Dousset, Anass Elhaddadi, Josiane Mothe </t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Dousset, Bernard and Elhaddadi, Anass and Mothe, Josiane},
+year = {2011},
+month = {12},
+pages = {},
+title = {Content Accessibility and Semantic Networks Processed on Foreign Natural Language Analysis},
+volume = {1},
+journal = {Journal of Intelligence Studies in Business}
+}</t>
+  </si>
+  <si>
+    <t>O autor sugere uma metodologia que possibilita a pesquisa documental em documentos distintos intependentemente da liguagem a qual o mesmo tenha sido escrito.</t>
+  </si>
+  <si>
+    <t>Early warning systems - Empirical evidence</t>
+  </si>
+  <si>
+    <t>Alexandra Rausch, Irene Fafaliou, Nidzara Osmanagic Bedenik</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Rausch, Alexandra and Fafaliou, Irene and Bedenik, Nidzara and Labas, Davor},
+year = {2012},
+month = {12},
+pages = {201-218},
+title = {Early warning systems - Empirical evidence},
+volume = {24},
+journal = {Review of Marketing Theory and Practice}
+}</t>
+  </si>
+  <si>
+    <t>Os autores informam que existe uma falta de evidências no que tange ao funcionamento empírico de sistemas de alertas antecipativos (early warning systems, em inglês), principalmente a nível de país. Assim os autores sugerem uma prática para verificar, em alguns países, os funcionamentos desse tipo de sistemas, levantando uma hipótese de que os sistemas existentes em países mais ricos, possuem esse tipo de sistema mais elaborado que em outros, chegando a níveis de estado da arte. O objetivo do artigo é preencher o espaço existente entre a exploração empírica de um EWS no que tange as suas características, importâncias e papeis em organizações existentes na Áustria, Croácia e Grécia.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Yoon, Janghyeok},
+year = {2012},
+month = {11},
+pages = {12543–12550},
+title = {Detecting weak signals for long-term business opportunities using text mining of Web news},
+volume = {39},
+journal = {Expert Systems with Applications},
+doi = {10.1016/j.eswa.2012.04.059}
+}</t>
+  </si>
+  <si>
+    <t>Detecting weak signals for long-term business opportunities using text mining of Web news</t>
+  </si>
+  <si>
+    <t>SISTEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUGERE MELHORIAS </t>
+  </si>
+  <si>
+    <t>POSSÍVEIS PROBLEMAS EXISTENTES PARA IMPLEMENTAR IC</t>
+  </si>
+  <si>
+    <t>POSSIBILIDADE DE METODOLOGIA</t>
+  </si>
+  <si>
+    <t>FORMA DE LEVANTAR SINAIS FRACOS</t>
+  </si>
+  <si>
+    <t>Propoe um método para buscar sinais fracos da web através de mineração de texto. O autor sugere como avaliação do método verificando notícias na web a respeito de placas solares. Os autores propões uma metodologia divida em três etapas: 1) coleta de notícias e/ou artigos; 2) definição de palavras-chave referentes a fatores ambientais, necessidades de negócio e componentes de produtos ou tecnológicos; 3) construção de um portfólio de palavras-chave evoluindo através do tempo (demonstrando o seu peso); e 4) identificação de tópicos de sinais fracos utilizando análise estatística e busca por notícias. O artigo fez uso de notícias estáticas, colocando como sugestão de trabalhos futuros, a utilização de web-crawlers em conjunto com text mining para fazer o levantamento desses sinais fracos.</t>
+  </si>
+  <si>
+    <t>THE SIGNIFICATION PROCESS OF THE FUTURE SIGN</t>
+  </si>
+  <si>
+    <t>SUGERE ENTENDER QUAIS SINAIS FRACOS SÃO NECESSÁRIO SEREM BUSCADOS.</t>
+  </si>
+  <si>
+    <t>Os autores propõem um framework para buscar o significado pleno dos sinais fracos (motivo da busca buscados, interpretação e produção).</t>
+  </si>
+  <si>
+    <t>Complexity science approaches to the application foresight</t>
+  </si>
+  <si>
+    <t>Os autores buscam com o seu trabalho tentar identificar possíveis tendências em 110 artigos da 20ª conferência do IPSERA (grupo de acadêmicos e praticantes em trocar ideias, estimular discussões e refletir em conceitos, teorias e formas/métodos educacionais de forma amigável) utilizando text mining.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Rozemeijer, Frank and Quintens, Lieven and Wetzels, Martin and Gelderman, Cees},
+year = {2012},
+month = {06},
+pages = {63–67},
+title = {Vision 20/20: Preparing today for tomorrow's challenges},
+volume = {18},
+journal = {Journal of Purchasing and Supply Management},
+doi = {10.1016/j.pursup.2012.04.005}
+}</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Kuusi, Osmo and Hiltunen, E.},
+year = {2012},
+month = {09},
+pages = {47-66},
+title = {The Signification Process of the Future Sign},
+volume = {16},
+journal = {Journal of Futures Studies}
+}</t>
+  </si>
+  <si>
+    <t>More applicable environmental scanning systems leveraging ‘‘modern’’ information systems</t>
+  </si>
+  <si>
+    <t>@article{2013MoreAE,
+  title={More applicable environmental scanning systems leveraging “modern” information systems},
+  author={},
+  journal={Information Systems and e-Business Management},
+  year={2013},
+  volume={11},
+  pages={507-540}
+}</t>
+  </si>
+  <si>
+    <t>SUGESTÃO DE COMO IMPLEMENTAR UM SISTEMA DE DETECÇÃO DE SINAIS FRACOS</t>
+  </si>
+  <si>
+    <t>Os autores informam que exisate um gap de informacional com relação a como um sistema de detecção de sinais fracos deveria funcionar. Sugerindo um guia conceitual para a criação de um sistema de escaneamento de ambiente. O processo que os autores propõem refere-se a uma implementação interna a uma organização.</t>
+  </si>
+  <si>
+    <t>Weak Signal identification with semantic web mining</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Thorleuchter, Dirk and Van den Poel, Dirk},
+year = {2013},
+month = {09},
+pages = {4978–4985},
+title = {Weak signal identification with semantic web mining},
+volume = {40},
+journal = {Expert Systems with Applications},
+doi = {10.1016/j.eswa.2013.03.002}
+}</t>
+  </si>
+  <si>
+    <t>Os autores implementam uma forma de busca de sinais fracos através da internet. Eles selecionaram previamente alguns websites relacionados com algumas hipóses que os mesmos criaram e utilizaram uma metodologia que utiliza indexação semantica latente (em inglês, LSI - latent semantic indexing). Segundo os autores, o LSI se baseia em aspectos para a criação de um entendimento naquilo que está sendo procurado, mesmo em contextos diferentes. Os autores informaram que, através dessa metodologia é possível calcular o maior número possível de sinais fracos relevantes representados pelas dimensões das decomposições de valor singular (em inglês, SVD - singular value decomposition).
+Os autores propõem como metodologia de trabalho a utilização combinada de classificação semântica de texto com mineração de dados automatizada para a busca e detecção de sinais fracos.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Dohn, Katarzyna and Gumiński, A. and Matusek, Mirosław and Zoleński, Wojciech},
+year = {2013},
+month = {01},
+pages = {211-221},
+title = {The early warning concept in the system supporting knowledge management in polish machine-building industry enterprises},
+journal = {Proceedings - KIM 2013, Knowledge and Information Management Conference: Sustainable Quality}
+}</t>
+  </si>
+  <si>
+    <t>The Early Warning Concept in the System Supporting Knowledge Management in Polish Machine-building Industry Enterprises</t>
+  </si>
+  <si>
+    <t>Os autores promovem uma discussão acerca daquilo que seria interessante abordar dentro de um sistema de avisos antecipativos (em inglês, EWS, early warning system).</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Thorleuchter, Dirk and Scheja, Tobias and Van den Poel, Dirk},
+year = {2014},
+month = {09},
+pages = {5009–5016},
+title = {Semantic weak signal tracing},
+volume = {41},
+journal = {Expert Systems with Applications},
+doi = {10.1016/j.eswa.2014.02.046}
+}</t>
+  </si>
+  <si>
+    <t>Semantic weak signal tracing</t>
+  </si>
+  <si>
+    <t>Os autores informam que a maioria dos trabalhos academicos com fins de buscar sinais fracos através da internet fazem isso através de uma análise textual dos documentos encontrados. Assim, eles fazem uma sugestão de nova metodologia que trabalha investigando uma sequência de clusters medidos em pontos sucessivos no tempo (series temporais), fazendo com que seja possível verificar uma evolução do sinal e, por fim, analisando sua real relevância. 
+Os autores também fazem uso de mineração e dados e buscam utilizar LSI, que é análise semantica do texto que está sendo buscado da internet.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Battistella, Cinzia},
+year = {2013},
+month = {01},
+pages = {},
+title = {The organisation of Corporate Foresight: A multiple case study in the telecommunication industry},
+volume = {87},
+journal = {Technological Forecasting and Social Change},
+doi = {10.1016/j.techfore.2013.10.022}
+}</t>
+  </si>
+  <si>
+    <t>The organisation of Corporate Foresight: A multiple case study in the telecommunication industry</t>
+  </si>
+  <si>
+    <t>FORMA DE IMPLEMENTAÇÃO DE UM CORPORATE FORESIGHT</t>
+  </si>
+  <si>
+    <t>Os autores buscam fazer uma avaliação das organizações caracterizadas como organizações com visão de futuro (em inglês, Corporate Foresight) afim de investigar como elas organizam a implementação de visão de futuro (corporate foresight). As dimensões organizacionais avaliadas são (estrutura organizacional, mecanismos de coordenação, processo de tomada de decisão e sistemas de controle) relacionando-as com medições de performance referentes a visão de futuro (CF) - eficiencia e efetividade.</t>
+  </si>
+  <si>
+    <t>Detecting Linguistic Markers for Radical Violence in Social Media</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Cohen, Katie and Johansson, Fredrik and Kaati, Lisa and Clausen Mork, Jonas},
+year = {2013},
+month = {12},
+pages = {2014},
+title = {Detecting Linguistic Markers for Radical Violence in Social Media},
+volume = {26},
+journal = {Terrorism and Political Violence},
+doi = {10.1080/09546553.2014.849948}
+}</t>
+  </si>
+  <si>
+    <t>Os autores buscam com o trabalho interceptar uma possível atividade terrorista feita pelos ditos "lone wolves terrorists" que são aqueles terroristas que agem por sua própria conta. Assim, eles propõem um método através da internet que busca por sinais fracos de possíveis atividades terroristas por acontecer. O método apresentado pelos autores é através de análise linguistica. Os autores usaram webcrawlers para buscar dados de forma automática e técnicas de análise textual (traduções, análise de sentimento, mapeamento de websites e reconhecimento de pessoas)  e análise de mídia social.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assessing emerging issues. The external and internal approach</t>
+  </si>
+  <si>
+    <t>Os autores tentam encontrar, em quaisquer tipos de questões existentes, características que possibilitem uma análise com fins de verificar a possibilidade de essas questões tornarem-se uma tendência relevante através do que eles chamam de perspectiva dupla. Essa perspectiva dupla coloca duas formas de avaliação, uma que envolve a questão em si e sua análise externa (do ambiente) e outra que envolve uma avaliação interna e a interpretação daqueles que as abordam.</t>
+  </si>
+  <si>
+    <t>SUGERE UM ENTENDIMENTO MELHOR ACERCA DOS SINAIS FRACOS</t>
+  </si>
+  <si>
+    <t>IT tools for foresight: The integrated insight and response system of Deutsche Telekom Innovation Laboratories</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Os autores fazem uma discussão de uma ferramenta desenvolvida pela Deutsche Telekom Ionnovation Laboratories para dar suporte em questões voltadas a visão de futuro. A ferramenta possui vários módulos e está vinculada diretamente com tomada de decisões da alta administração. A ferramenta possui módulos referentes à descoberta de mudanças, interpretações, auxílio à respostas rápidas (gerenciais), gestão de ideias internas à organização e uma abordagem de escaneamento e gestão de sinais fracos. 
+Existem 3 processos de visão de futuro que o sistema aborda: i) Coleta de dados tanto internos quanto externos, através de ideias, observações, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insights</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, etc); ii) Interpretação, fazendo com que vários interessados possam analisar e julgar informações sob a sua própria perspectiva ou mesmo entrar em contato com outros interessados (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stakeholders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">); e iii) Respostas organizacionais. 
+Existem 3 plataformas integradas que fazem o suporte de visão de futuro: i) PEACOQ Scouting Tool que é uma ferramenta que faz o escaneamento ambiental de tendências; ii) PEACOQ Gate 0.5 que é um ambiente de ideação, com fins de criação e gestão de ideias; e iii) Intranet, que é um local para desenvolvimento de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insights</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Rohrbeck, René and Thom, Nico and Arnold, Heinrich},
+year = {2015},
+month = {08},
+pages = {115-126},
+title = {IT Tools for Foresight: The Integrated Insight and Response System of Deutsche Telekom Innovation Laboratories},
+volume = {97},
+journal = {Technological Forecasting and Social Change},
+doi = {10.1016/j.techfore.2013.09.015}
+}</t>
+  </si>
+  <si>
+    <t>A foresight toolkit for smart specialization and entrepreneurial discovery</t>
+  </si>
+  <si>
+    <t>Os autores sugerem uma forma de busca e classificação de sinais fracos semi-automática. Um sistema busca possíveis sinais fracos e os cadastram em um portal. Uma vez cadastrados, pessoas fazem a avaliação desses possíveis sinais fracos com o intuito de classificá-los. Algumas vezes pode ocorrer de grupos se reunirem para debater sobre um determinado ou determinados sinais, mantendo-os em evolução na ferramenta. Os autores não dão detalhes acerca de tecnologias utilizadas.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Gheorghiu, Radu and Andreescu, Liviu and Curaj, Adrian},
+year = {2016},
+month = {04},
+pages = {},
+title = {A foresight toolkit for smart specialization and entrepreneurial discovery},
+journal = {Futures},
+doi = {10.1016/j.futures.2016.04.001}
+}</t>
+  </si>
+  <si>
+    <t>CONCEPTION OF A KNOWLEDGE MANAGEMENT SYSTEM FOR TECHNOLOGIES</t>
+  </si>
+  <si>
+    <t>Os autores apresentam uma solução de software que faz uso da internet para buscar novas tendencias de tecnologias. O software faz uso de mineração de texto através de um robo (web crawler) que busca essas tendências a partir de uma instrução de busca inserida manualmente.</t>
+  </si>
+  <si>
+    <t>@inproceedings{placzek2015conception,
+  title={Conception of a knowledge management system for technologies},
+  author={Placzek, Markus and Eberling, Christian and Gausemeier, J{\"u}rgen},
+  booktitle={24th International Association for Management of Technology Conference Proceedings, Cape Town},
+  pages={16461663},
+  year={2015}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SISTEMA </t>
+  </si>
+  <si>
+    <t>A visual scanning of potential disruptive signals for technology roadmapping: investigating keyword cluster, intensity, and relationship in futuristic data</t>
+  </si>
+  <si>
+    <t>Os autores sugerem uma forma nova de buscar identificar tecnologias disruptivas. Ao invés de buscarem sempre informações em websites de patentes que, como colocado pelos autores, informa somente uma possível trajetória da tecnologia, os mesmos sugerem o desenvolvimento de um sistema de suporte a decisão com fins de buscar um roadmapping de tecnologias futuras, fazendo uso de tendências e mega tendências encontradas na inetrnet. Os autores farão uso de tecnologias de mineração de texto e algoritmos de visualização de informação e mapas contendo palavras-chave para as possíveis áreas de disrupção tecnológica, possíveis sinais disruptivos  e os possíveis caminhos para se chegar a essas disrupções.</t>
+  </si>
+  <si>
+    <t>@article{kim2016visual,
+  title={A visual scanning of potential disruptive signals for technology roadmapping: investigating keyword cluster, intensity, and relationship in futuristic data},
+  author={Kim, Jieun and Park, Yongtae and Lee, Youngjo},
+  journal={Technology Analysis \&amp; Strategic Management},
+  volume={28},
+  number={10},
+  pages={1225--1246},
+  year={2016},
+  publisher={Taylor \&amp; Francis}
+}</t>
+  </si>
+  <si>
+    <t>Identification of Potential Collective Actions using
+Enhanced Gray System Theory on Social Media</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Os autores propõem uma forma de identificar possíveis ações coletivas iniciadas por usuários nas redes sociais e que são compartilhadas entre outros usuários. O objetivo é fazer com qua autoridades consigam adiantar ações ao perceber sinais fracos de possíveis levantes. Os autores fizeram uso de ferramentas de análise de sentimentos para identificar o tipo de sinal que está sendo avaliado. Os autores não discutiram formas de buscar os possíveis sinais fracos, recuperando as informações de protestos por meio de uma ferramenta que armazena histórico de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tweets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>@article{yang2016identification,
+  title={Identification of Potential Collective Actions Using Enhanced Gray System Theory on Social Media},
+  author={Yang, Wei and Cui, Xiaohui and Liu, Jin and Liu, Yancheng},
+  journal={IEEE Access},
+  volume={4},
+  pages={9184--9192},
+  year={2016},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>IDENTIFYING AND EVALUATING DISRUPTIVE TECHNOLOGIES USING TECHNOLOGY SCANNING</t>
+  </si>
+  <si>
+    <t>SISTEMA BUSCAR TECNOLOGIAS DISRUPTIVAS</t>
+  </si>
+  <si>
+    <t>SISTEMA BUSCAR TECNOLOGIAS DISRUPTIVAS (processo, sem informações acerca de implementações)</t>
+  </si>
+  <si>
+    <r>
+      <t>Os autores buscam demonstram um framwork com fins de buscar identificar sinais fracos com relação à tendências tecnológicas. Os autores utilizam uma ferramenta que possui uma série de métodos de "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>foresight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" como </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>forecasting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, análise de cenário, métodos de análise de tendências. Não entram na quesão tecnológica, mas elaboram um processo com alguns requisitos importantes acerca da implantação de um sistema de escaneamento tecnológico.</t>
+    </r>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>@article{carbonell2015assessing,
+  title={Assessing emerging issues. The external and internal approach},
+  author={Carbonell, Javier and S{\'a}nchez-Esguevillas, Antonio and Carro, Bel{\'e}n},
+  journal={Futures},
+  volume={73},
+  pages={12--21},
+  year={2015},
+  publisher={Elsevier}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{Schuh2016IdentifyingAE,
+  title={Identifying and Evaluating Disruptive Technologies Using Technology Scanning},
+  author={Guenther Schuh and Toni Drescher and Patrick Kabasci and S. Ryschka and Tim Wetterney},
+  year={2016}
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,13 +714,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,18 +749,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,100 +1089,594 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5CE23C-BB8F-374F-A4F3-25FE445B638E}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="H18" sqref="A17:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="18.83203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="43.83203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="68" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="28" style="3" customWidth="1"/>
+    <col min="6" max="6" width="71.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="154" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="3">
         <v>2009</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="3">
         <v>2009</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="150" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="3">
+        <v>2010</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2011</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2011</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2011</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2012</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2014</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2014</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2015</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2011</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2012</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="C26" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H26" xr:uid="{5354611A-11CC-164A-992F-3466BA84A058}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H26">
+      <sortCondition ref="H1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parte final para a qualificação
</commit_message>
<xml_diff>
--- a/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
+++ b/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C02841-CBFD-8542-AAA3-932085ED817A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D3CDA1-6CF5-454C-A94A-EC8FC3D95CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
   </bookViews>
@@ -288,18 +288,6 @@
   </si>
   <si>
     <t>Os autores buscam com o seu trabalho tentar identificar possíveis tendências em 110 artigos da 20ª conferência do IPSERA (grupo de acadêmicos e praticantes em trocar ideias, estimular discussões e refletir em conceitos, teorias e formas/métodos educacionais de forma amigável) utilizando text mining.</t>
-  </si>
-  <si>
-    <t>@article{article,
-author = {Rozemeijer, Frank and Quintens, Lieven and Wetzels, Martin and Gelderman, Cees},
-year = {2012},
-month = {06},
-pages = {63–67},
-title = {Vision 20/20: Preparing today for tomorrow's challenges},
-volume = {18},
-journal = {Journal of Purchasing and Supply Management},
-doi = {10.1016/j.pursup.2012.04.005}
-}</t>
   </si>
   <si>
     <t>@article{article,
@@ -689,6 +677,18 @@
   year={2016}
 }</t>
   </si>
+  <si>
+    <t>@article{article,
+author = {Horton, Averil},
+year = {2012},
+month = {07},
+pages = {294-303},
+title = {Complexity science approaches to the application foresight},
+volume = {14},
+journal = {foresight},
+doi = {10.1108/14636681211256080}
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -749,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -774,6 +774,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5CE23C-BB8F-374F-A4F3-25FE445B638E}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="H18" sqref="A17:H18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="89" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1133,24 +1136,24 @@
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="6">
         <v>2014</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
@@ -1247,7 +1250,7 @@
       <c r="E6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="6">
@@ -1257,7 +1260,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -1326,9 +1329,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>56</v>
@@ -1348,18 +1351,18 @@
     </row>
     <row r="11" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="6">
         <v>2013</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -1370,18 +1373,18 @@
     </row>
     <row r="12" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="6">
         <v>2014</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
@@ -1392,18 +1395,18 @@
     </row>
     <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="6">
         <v>2014</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" s="6">
         <v>1</v>
@@ -1414,18 +1417,18 @@
     </row>
     <row r="14" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="6">
         <v>2015</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -1436,16 +1439,16 @@
     </row>
     <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" s="3">
         <v>2016</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1456,64 +1459,64 @@
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3">
         <v>2015</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="G17" s="3">
         <v>1</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="3">
         <v>2016</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G18" s="3">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>53</v>
@@ -1583,91 +1586,91 @@
     </row>
     <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3">
         <v>2015</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="G22" s="3">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="6">
         <v>2013</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="6">
         <v>1</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="6">
         <v>2013</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="6">
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="3">
         <v>2015</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="C26" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leitura da revisão de literatura
</commit_message>
<xml_diff>
--- a/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
+++ b/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/Fichamento.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D3CDA1-6CF5-454C-A94A-EC8FC3D95CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1000A7E0-7FDD-CF4E-BEB9-AB497BEB055C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
+    <workbookView xWindow="-4980" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{E0C950AB-5085-2340-8F25-0885C4924BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="001_2011" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$H$26</definedName>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
   <si>
     <t>@article{article,
 author = {Rossel, Pierre},
@@ -689,12 +691,117 @@
 doi = {10.1108/14636681211256080}
 }</t>
   </si>
+  <si>
+    <t>Environmental Scanning Systems: State of the art and first instantiation</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Metodologia</t>
+  </si>
+  <si>
+    <t>Pontos de Discussão</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
+  </si>
+  <si>
+    <t>Problema</t>
+  </si>
+  <si>
+    <t>A dificuldade em colocar em prática (operacionalizar) os conceitos de ESS existentes.</t>
+  </si>
+  <si>
+    <t>Fazer um levantamento de ESS existente na literatura e suas principais implementacoes.</t>
+  </si>
+  <si>
+    <t>Dividiu a pesquisa em 2 pontos: elementos que caracterizam o desenvolvimento de um sistema de informação e elementos que caracterizam a pesquisa feita (método de pesquisa). 
+Para o primeiro, o autor dividiu em 3 pontos, requisitos de usuário, que caracteriza aquilo que o sistema deverá fazer (requisitos funcionais e não funcionais), modelos, dividido em forecasting, indicadores ou environmental scanning using weak signals e métodos que demonstram como o sistema alcançaria o seu objetivo, através de uma junção de informações (scanning), técnicas analíticas para identificar mudanças latentes ou pendentes ou a incorporação do resultado do scaneamento no processo de tomada de decisões dos executivos.
+Para o segundo ele dividiu em modo empírico que foi dividido em estudos de caso, experimentos e surveys e desenho (design) que por sua vez foi dividido em lista de requisitos e framework que faz uma ligação entre requisitos e princípios de design.</t>
+  </si>
+  <si>
+    <t>REQUISITOS DO USUÁRIOS - PRIMEIRO ACHADO
+Por conta da necessidade que os executivos possuem de gerenciar uma companhina de forma geral, sugere-se o desenvolvimento de um "radar 360º". Este radar deverá refletir a estratégia da organização, priorizando as áreas de escanemanto de acordo com a sua cadeia de valor. As mais importantes áreas são oferta de capital, pesquisa e desenvolvimento e recursos humanos. Para empresas mais voláteis é importante também atentarem-se a cientica, política, leis e justiça e relações internacionais.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MODELOS - TERCEIRO ACHADO
+Alavancar a TI para automatizar rotinas de trabalho diárias e seguir o movimento dos indicadores. É importante que sejam definidas as fontes de onde serão monitoradas as informações. Essas fontes podem ser a própria Internet ou Mercado de Capitais. Como sugestão pela facilidade na manipulação, sugere-se a utlização de linguagens como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XBRL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (eXtensible Business Reporting Language) para facilitar essa automatização de rotinas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MODELOS - SEGUNDO ACHADO
+Definir indicadores concretos e usar TI para identificar cadeias relevantes de causa e efeito. Para isso é importante que seja possível distinguir dentre a grande quantidade de dados existentes aqueles indicadores que possuem uma característica relevantes de mudança, como critéria de avaliação dos indicadores são sugeridos lead time, clarificação e a proporção do custo/impacto. Também é importante se apropriar da tecnologia da informação para extrair essa cadeia de causa e efeito através de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>estrutuação de dados, redes neurais artificiais, mineração de dados, e busca semantica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Elofson &amp; Konsynski 1991).</t>
+    </r>
+  </si>
+  <si>
+    <t>MÉTODOS - QUARTO ACHADO
+Alavancar experiências de alto nível com uma matriz de impacto e traduzir indicadores de impacto em um portifólio de oportunidades e ameaçar balanceado. Utilizar ferramentas como método Delphi e Cross Impact Analysis (Mayer &amp; Wurl 2011).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MÉTODOS - QUINTO ACHADO
+Incorporar resultados do trabalho de escaneamento nos processos de tomada de decisão dos executivos através da geração de cenários através de uma certa quantidade de hipóteses. </t>
+  </si>
+  <si>
+    <t>MÉTODOS - SEXTO ACHADO
+Utilize controles retrospectivos para continuamente atualizar o sistema e colaborar para o compartilhamento de achados (escaneados) nos trabalhos do dia-a-dia. Além de relatórios improvisados (ad hoc), é interessante que, periodicamente, um relatório que contenha os achados do período seja desenvolvido pra que possíveis cenários sejam vislumbrados.</t>
+  </si>
+  <si>
+    <t>Propõem que sejam utilizado Redes Neurais Artificiais como forma de implementar capacidades de busca de sinais antecipativos nas corporações. Justificando que, ao contrário dos bumanos, as redes neurais não tem limitações psicológicas além de terem a capacidade de tratar várias variáveis ao mesmo tempo.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -717,6 +824,14 @@
     <font>
       <i/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -749,7 +864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -777,6 +892,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,13 +1224,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5CE23C-BB8F-374F-A4F3-25FE445B638E}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="89" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A17" zoomScale="114" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68" style="4" customWidth="1"/>
+    <col min="1" max="1" width="101.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="3"/>
@@ -1682,4 +1812,505 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC2757D-42FD-B54E-9A86-C420C271047C}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="81.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="135" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="135" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2011</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2012</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2012</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="195" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2012</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2012</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2013</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2014</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="270" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2014</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2015</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2016</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="165" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H17">
+    <sortCondition ref="D2"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB970C8-7D77-9141-915A-E8FF08EBA83D}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="34.83203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="65.1640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="67.6640625" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="E3" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="F4" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="F5" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="F6" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="F7" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="F8" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="F9" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>